<commit_message>
push final mark history by BY output file
</commit_message>
<xml_diff>
--- a/outputs/R_OUT - San Juan mark history by BROOD YEAR.xlsx
+++ b/outputs/R_OUT - San Juan mark history by BROOD YEAR.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:Q44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,47 +365,47 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>total_oto_release</t>
+          <t>TM_release</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>RF READ STATUS</t>
+          <t>TM_read_status</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>TM_application_flag</t>
+          <t>n_submitted_refSpec_by_BY</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>total_oto_refs</t>
+          <t>TM Quality (%): NA</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>TM Quality (%): Unknown</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>TM Quality (%): Good</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Acceptable</t>
+          <t>TM Quality (%): Acceptable</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Poor</t>
+          <t>TM Quality (%): Poor</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>BY total released</t>
+          <t>SEP_released</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -431,76 +431,45 @@
       <c r="O1" s="1" t="inlineStr">
         <is>
           <t>total_rel_check</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>PBT</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>TM_comments</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2">
-        <v>2001</v>
-      </c>
-      <c r="B2">
-        <v>785000</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
+        <v>1979</v>
       </c>
       <c r="J2">
-        <v>785000</v>
+        <v>39555</v>
       </c>
       <c r="K2">
-        <v>0.096</v>
+        <v>0.989</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="M2">
-        <v>0.096</v>
+        <v>0.994</v>
       </c>
       <c r="N2">
-        <v>0.904</v>
-      </c>
-      <c r="O2" t="b">
-        <v>1</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2002</v>
-      </c>
-      <c r="B3">
-        <v>772052</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
+        <v>1980</v>
       </c>
       <c r="J3">
-        <v>772052</v>
+        <v>5560</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -512,121 +481,55 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>2003</v>
-      </c>
-      <c r="B4">
-        <v>1074172</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
+        <v>1981</v>
       </c>
       <c r="J4">
-        <v>1074172</v>
+        <v>187527</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>0.55</v>
       </c>
       <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4" t="b">
-        <v>1</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>2004</v>
-      </c>
-      <c r="B5">
-        <v>1000000</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
+        <v>1982</v>
       </c>
       <c r="J5">
-        <v>1000000</v>
+        <v>148677</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>0.335</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>0.348</v>
       </c>
       <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5" t="b">
-        <v>1</v>
+        <v>0.652</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>2005</v>
-      </c>
-      <c r="B6">
-        <v>373275</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
+        <v>1983</v>
       </c>
       <c r="J6">
-        <v>373275</v>
+        <v>99452</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -638,37 +541,15 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="O6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>2006</v>
-      </c>
-      <c r="B7">
-        <v>985155</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
+        <v>1984</v>
       </c>
       <c r="J7">
-        <v>985155</v>
+        <v>367000</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -680,37 +561,15 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="O7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>2007</v>
-      </c>
-      <c r="B8">
-        <v>518510</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
+        <v>1985</v>
       </c>
       <c r="J8">
-        <v>518510</v>
+        <v>29700</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -722,37 +581,15 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>1</v>
-      </c>
-      <c r="O8" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>2008</v>
-      </c>
-      <c r="B9">
-        <v>945650</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
+        <v>1986</v>
       </c>
       <c r="J9">
-        <v>945650</v>
+        <v>300325</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -764,108 +601,55 @@
         <v>0</v>
       </c>
       <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="O9" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>2009</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
+        <v>1987</v>
       </c>
       <c r="J10">
-        <v>1038800</v>
+        <v>711091</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>0.147</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>0.148</v>
       </c>
       <c r="N10">
-        <v>1</v>
-      </c>
-      <c r="O10" t="b">
-        <v>0</v>
+        <v>0.852</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>2010</v>
-      </c>
-      <c r="B11">
-        <v>840000</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>mark application issue: actual mark applied was not the intended mark applied</t>
-        </is>
-      </c>
-      <c r="E11">
-        <v>28</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
+        <v>1988</v>
       </c>
       <c r="J11">
-        <v>840000</v>
+        <v>678464</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>0.153</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>0.155</v>
       </c>
       <c r="N11">
-        <v>1</v>
-      </c>
-      <c r="O11" t="b">
-        <v>1</v>
+        <v>0.845</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>2011</v>
-      </c>
-      <c r="B12">
-        <v>245000</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="E12">
-        <v>14</v>
-      </c>
-      <c r="G12">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="H12">
-        <v>0.93</v>
+        <v>1990</v>
       </c>
       <c r="J12">
-        <v>245000</v>
+        <v>158990</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -877,37 +661,15 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <v>1</v>
-      </c>
-      <c r="O12" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>2012</v>
-      </c>
-      <c r="B13">
-        <v>1031800</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>mark application issue: actual mark applied was not the intended mark applied</t>
-        </is>
-      </c>
-      <c r="E13">
-        <v>10</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
+        <v>1991</v>
       </c>
       <c r="J13">
-        <v>1031800</v>
+        <v>625000</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -919,125 +681,75 @@
         <v>0</v>
       </c>
       <c r="N13">
-        <v>1</v>
-      </c>
-      <c r="O13" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>2013</v>
-      </c>
-      <c r="B14">
-        <v>319000</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>mark application issue: actual mark applied was not the intended mark applied</t>
-        </is>
-      </c>
-      <c r="E14">
-        <v>10</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
+        <v>1992</v>
       </c>
       <c r="J14">
-        <v>319000</v>
+        <v>353071</v>
       </c>
       <c r="K14">
-        <v>0.141</v>
+        <v>0.385</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>0.141</v>
+        <v>0.385</v>
       </c>
       <c r="N14">
-        <v>0.859</v>
-      </c>
-      <c r="O14" t="b">
-        <v>1</v>
+        <v>0.615</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>2015</v>
+        <v>1993</v>
       </c>
       <c r="J15">
-        <v>219352</v>
+        <v>1130250</v>
       </c>
       <c r="K15">
-        <v>0.203</v>
+        <v>0.045</v>
       </c>
       <c r="L15">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="M15">
-        <v>0.204</v>
+        <v>0.045</v>
       </c>
       <c r="N15">
-        <v>0.796</v>
+        <v>0.955</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>2017</v>
-      </c>
-      <c r="B16">
-        <v>249899</v>
+        <v>1994</v>
       </c>
       <c r="J16">
-        <v>249899</v>
+        <v>670000</v>
       </c>
       <c r="K16">
-        <v>0.18</v>
+        <v>0.076</v>
       </c>
       <c r="L16">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="M16">
-        <v>0.182</v>
+        <v>0.076</v>
       </c>
       <c r="N16">
-        <v>0.8179999999999999</v>
-      </c>
-      <c r="O16" t="b">
-        <v>1</v>
+        <v>0.924</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>2018</v>
-      </c>
-      <c r="B17">
-        <v>66794</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="E17">
-        <v>10</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
+        <v>1995</v>
       </c>
       <c r="J17">
-        <v>66794</v>
+        <v>600000</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -1049,40 +761,15 @@
         <v>0</v>
       </c>
       <c r="N17">
-        <v>1</v>
-      </c>
-      <c r="O17" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>2019</v>
-      </c>
-      <c r="B18">
-        <v>184597</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>mark application issue: actual mark applied was not the intended mark applied</t>
-        </is>
-      </c>
-      <c r="E18">
-        <v>10</v>
-      </c>
-      <c r="G18">
-        <v>0.9</v>
-      </c>
-      <c r="H18">
-        <v>0.1</v>
+        <v>1996</v>
       </c>
       <c r="J18">
-        <v>184597</v>
+        <v>410000</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -1094,21 +781,15 @@
         <v>0</v>
       </c>
       <c r="N18">
-        <v>1</v>
-      </c>
-      <c r="O18" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>2020</v>
-      </c>
-      <c r="B19">
-        <v>422512</v>
+        <v>1997</v>
       </c>
       <c r="J19">
-        <v>422512</v>
+        <v>275000</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -1120,140 +801,209 @@
         <v>0</v>
       </c>
       <c r="N19">
-        <v>1</v>
-      </c>
-      <c r="O19" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>2021</v>
-      </c>
-      <c r="B20">
-        <v>500039</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="E20">
-        <v>9</v>
-      </c>
-      <c r="I20">
-        <v>1</v>
+        <v>1998</v>
       </c>
       <c r="J20">
-        <v>500039</v>
+        <v>1275000</v>
       </c>
       <c r="K20">
-        <v>0.075</v>
+        <v>0</v>
       </c>
       <c r="L20">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="M20">
-        <v>0.08599999999999999</v>
+        <v>0</v>
       </c>
       <c r="N20">
-        <v>0.914</v>
-      </c>
-      <c r="O20" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>1979</v>
+        <v>1999</v>
       </c>
       <c r="J21">
-        <v>39555</v>
+        <v>850000</v>
       </c>
       <c r="K21">
-        <v>0.989</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="L21">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="M21">
-        <v>0.994</v>
+        <v>0.089</v>
       </c>
       <c r="N21">
-        <v>0.006</v>
+        <v>0.911</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>1980</v>
+        <v>2000</v>
       </c>
       <c r="J22">
-        <v>5560</v>
+        <v>224429</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>0.336</v>
       </c>
       <c r="L22">
         <v>0</v>
       </c>
       <c r="M22">
-        <v>0</v>
+        <v>0.336</v>
       </c>
       <c r="N22">
-        <v>1</v>
+        <v>0.664</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>1981</v>
+        <v>2001</v>
+      </c>
+      <c r="B23">
+        <v>785000</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Marked</t>
+        </is>
+      </c>
+      <c r="D23">
+        <v>16</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
       </c>
       <c r="J23">
-        <v>187527</v>
+        <v>785000</v>
       </c>
       <c r="K23">
-        <v>0.52</v>
+        <v>0.096</v>
       </c>
       <c r="L23">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="M23">
-        <v>0.55</v>
+        <v>0.096</v>
       </c>
       <c r="N23">
-        <v>0.45</v>
+        <v>0.904</v>
+      </c>
+      <c r="O23" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>READS WERE 2:1.4+2.2 FOR 16 SAMPLES</t>
+        </is>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>1982</v>
+        <v>2002</v>
+      </c>
+      <c r="B24">
+        <v>772052</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Marked</t>
+        </is>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
       </c>
       <c r="J24">
-        <v>148677</v>
+        <v>772052</v>
       </c>
       <c r="K24">
-        <v>0.335</v>
+        <v>0</v>
       </c>
       <c r="L24">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="M24">
-        <v>0.348</v>
+        <v>0</v>
       </c>
       <c r="N24">
-        <v>0.652</v>
+        <v>1</v>
+      </c>
+      <c r="O24" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>NO REFERENCE SAMPLES.   RELEASE OF PINHEADS RESULTING FROM POOR FEED QUALITY-EWOS / NO REFERENCE SAMPLES.   FED FRY RELEASE, NO REFERENCE SAMPLES.</t>
+        </is>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>1983</v>
+        <v>2003</v>
+      </c>
+      <c r="B25">
+        <v>1074172</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Marked</t>
+        </is>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
       </c>
       <c r="J25">
-        <v>99452</v>
+        <v>1074172</v>
       </c>
       <c r="K25">
         <v>0</v>
@@ -1266,14 +1016,48 @@
       </c>
       <c r="N25">
         <v>1</v>
+      </c>
+      <c r="O25" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>NO SAMPLE RECEIVED</t>
+        </is>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>1984</v>
+        <v>2004</v>
+      </c>
+      <c r="B26">
+        <v>1000000</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Marked</t>
+        </is>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
       </c>
       <c r="J26">
-        <v>367000</v>
+        <v>1000000</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -1286,14 +1070,48 @@
       </c>
       <c r="N26">
         <v>1</v>
+      </c>
+      <c r="O26" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>12 HOUR THERMAL CYCLE NO SAMPLE RECEIVED</t>
+        </is>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>1985</v>
+        <v>2005</v>
+      </c>
+      <c r="B27">
+        <v>373275</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Marked</t>
+        </is>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
       </c>
       <c r="J27">
-        <v>29700</v>
+        <v>373275</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -1306,14 +1124,48 @@
       </c>
       <c r="N27">
         <v>1</v>
+      </c>
+      <c r="O27" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>12 HOUR THERMAL CYCLE NO SAMPLE RECEIVED</t>
+        </is>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>1986</v>
+        <v>2006</v>
+      </c>
+      <c r="B28">
+        <v>985155</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Marked</t>
+        </is>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
       </c>
       <c r="J28">
-        <v>300325</v>
+        <v>985155</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -1326,54 +1178,156 @@
       </c>
       <c r="N28">
         <v>1</v>
+      </c>
+      <c r="O28" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>NO SAMPLE 12 HOUR THERMAL CYCLE</t>
+        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>1987</v>
+        <v>2007</v>
+      </c>
+      <c r="B29">
+        <v>518510</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Marked</t>
+        </is>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
       </c>
       <c r="J29">
-        <v>711091</v>
+        <v>518510</v>
       </c>
       <c r="K29">
-        <v>0.147</v>
+        <v>0</v>
       </c>
       <c r="L29">
         <v>0</v>
       </c>
       <c r="M29">
-        <v>0.148</v>
+        <v>0</v>
       </c>
       <c r="N29">
-        <v>0.852</v>
+        <v>1</v>
+      </c>
+      <c r="O29" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>NO REFERENCE SAMPLE. THERMAL RECORDS PROVIDED BY HATCHERY</t>
+        </is>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>1988</v>
+        <v>2008</v>
+      </c>
+      <c r="B30">
+        <v>945650</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Marked</t>
+        </is>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
       </c>
       <c r="J30">
-        <v>678464</v>
+        <v>945650</v>
       </c>
       <c r="K30">
-        <v>0.153</v>
+        <v>0</v>
       </c>
       <c r="L30">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="M30">
-        <v>0.155</v>
+        <v>0</v>
       </c>
       <c r="N30">
-        <v>0.845</v>
+        <v>1</v>
+      </c>
+      <c r="O30" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>NO SAMPLE BUT THERMAL RECORDS(COHO POSSIBLY INCIDENTALLY MARKED)</t>
+        </is>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>1990</v>
+        <v>2009</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Not Marked</t>
+        </is>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
       </c>
       <c r="J31">
-        <v>158990</v>
+        <v>1038800</v>
       </c>
       <c r="K31">
         <v>0</v>
@@ -1386,14 +1340,48 @@
       </c>
       <c r="N31">
         <v>1</v>
+      </c>
+      <c r="O31" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>FOUR MILE HATCHERY NO SAMPLE - MAURICE TREMBLAY NOT MARKED THIS YEAR DUE TO WATER TEMPERATURE ISSUES (SEE NOCN09115 AND NOCN09103)1,038,800 NOT THERMALLY MARKED.</t>
+        </is>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>1991</v>
+        <v>2010</v>
+      </c>
+      <c r="B32">
+        <v>840000</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Marked</t>
+        </is>
+      </c>
+      <c r="D32">
+        <v>35</v>
+      </c>
+      <c r="E32">
+        <v>0.2</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0.8</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
       </c>
       <c r="J32">
-        <v>625000</v>
+        <v>840000</v>
       </c>
       <c r="K32">
         <v>0</v>
@@ -1406,232 +1394,640 @@
       </c>
       <c r="N32">
         <v>1</v>
+      </c>
+      <c r="O32" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>mark application issue: actual mark applied was not the intended mark applied</t>
+        </is>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>1992</v>
+        <v>2011</v>
+      </c>
+      <c r="B33">
+        <v>245000</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Marked</t>
+        </is>
+      </c>
+      <c r="D33">
+        <v>15</v>
+      </c>
+      <c r="E33">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="H33">
+        <v>0.87</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
       </c>
       <c r="J33">
-        <v>353071</v>
+        <v>245000</v>
       </c>
       <c r="K33">
-        <v>0.385</v>
+        <v>0</v>
       </c>
       <c r="L33">
         <v>0</v>
       </c>
       <c r="M33">
-        <v>0.385</v>
+        <v>0</v>
       </c>
       <c r="N33">
-        <v>0.615</v>
+        <v>1</v>
+      </c>
+      <c r="O33" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>1993</v>
+        <v>2012</v>
+      </c>
+      <c r="B34">
+        <v>1031800</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Marked</t>
+        </is>
+      </c>
+      <c r="D34">
+        <v>10</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
       </c>
       <c r="J34">
-        <v>1130250</v>
+        <v>1031800</v>
       </c>
       <c r="K34">
-        <v>0.045</v>
+        <v>0</v>
       </c>
       <c r="L34">
         <v>0</v>
       </c>
       <c r="M34">
-        <v>0.045</v>
+        <v>0</v>
       </c>
       <c r="N34">
-        <v>0.955</v>
+        <v>1</v>
+      </c>
+      <c r="O34" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>mark application issue: actual mark applied was not the intended mark applied</t>
+        </is>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>1994</v>
+        <v>2013</v>
+      </c>
+      <c r="B35">
+        <v>319000</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Marked</t>
+        </is>
+      </c>
+      <c r="D35">
+        <v>10</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
       </c>
       <c r="J35">
-        <v>670000</v>
+        <v>319000</v>
       </c>
       <c r="K35">
-        <v>0.076</v>
+        <v>0.141</v>
       </c>
       <c r="L35">
         <v>0</v>
       </c>
       <c r="M35">
-        <v>0.076</v>
+        <v>0.141</v>
       </c>
       <c r="N35">
-        <v>0.924</v>
+        <v>0.859</v>
+      </c>
+      <c r="O35" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>mark application issue: actual mark applied was not the intended mark applied</t>
+        </is>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>1995</v>
+        <v>2014</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Not Marked</t>
+        </is>
+      </c>
+      <c r="D36">
+        <v>17</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
       </c>
       <c r="J36">
-        <v>600000</v>
+        <v>237435</v>
       </c>
       <c r="K36">
-        <v>0</v>
+        <v>0.158</v>
       </c>
       <c r="L36">
         <v>0</v>
       </c>
       <c r="M36">
-        <v>0</v>
+        <v>0.158</v>
       </c>
       <c r="N36">
-        <v>1</v>
+        <v>0.842</v>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>mark application issue: actual mark applied was not the intended mark applied</t>
+        </is>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>1996</v>
+        <v>2015</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Not Marked</t>
+        </is>
+      </c>
+      <c r="D37">
+        <v>10</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
       </c>
       <c r="J37">
-        <v>410000</v>
+        <v>219352</v>
       </c>
       <c r="K37">
-        <v>0</v>
+        <v>0.203</v>
       </c>
       <c r="L37">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="M37">
-        <v>0</v>
+        <v>0.204</v>
       </c>
       <c r="N37">
-        <v>1</v>
+        <v>0.796</v>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>mark application issue: actual mark applied was not the intended mark applied</t>
+        </is>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>1997</v>
+        <v>2016</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Not Marked</t>
+        </is>
+      </c>
+      <c r="D38">
+        <v>10</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
       </c>
       <c r="J38">
-        <v>275000</v>
+        <v>542856</v>
       </c>
       <c r="K38">
-        <v>0</v>
+        <v>0.089</v>
       </c>
       <c r="L38">
         <v>0</v>
       </c>
       <c r="M38">
-        <v>0</v>
+        <v>0.089</v>
       </c>
       <c r="N38">
-        <v>1</v>
+        <v>0.911</v>
+      </c>
+      <c r="O38" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>mark application issue: actual mark applied was not the intended mark applied</t>
+        </is>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>1998</v>
+        <v>2017</v>
+      </c>
+      <c r="B39">
+        <v>249899</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Not Marked</t>
+        </is>
+      </c>
+      <c r="D39">
+        <v>10</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
       </c>
       <c r="J39">
-        <v>1275000</v>
+        <v>249899</v>
       </c>
       <c r="K39">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="L39">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="M39">
-        <v>0</v>
+        <v>0.182</v>
       </c>
       <c r="N39">
-        <v>1</v>
+        <v>0.8179999999999999</v>
+      </c>
+      <c r="O39" t="b">
+        <v>1</v>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>Incomplete</t>
+        </is>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>mark application issue: actual mark applied was not the intended mark applied</t>
+        </is>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>1999</v>
+        <v>2018</v>
+      </c>
+      <c r="B40">
+        <v>66794</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Marked</t>
+        </is>
+      </c>
+      <c r="D40">
+        <v>10</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
       </c>
       <c r="J40">
-        <v>850000</v>
+        <v>66794</v>
       </c>
       <c r="K40">
-        <v>0.08799999999999999</v>
+        <v>0</v>
       </c>
       <c r="L40">
         <v>0</v>
       </c>
       <c r="M40">
-        <v>0.089</v>
+        <v>0</v>
       </c>
       <c r="N40">
-        <v>0.911</v>
+        <v>1</v>
+      </c>
+      <c r="O40" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
       </c>
     </row>
     <row r="41">
       <c r="A41">
-        <v>2000</v>
+        <v>2019</v>
+      </c>
+      <c r="B41">
+        <v>184597</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Marked</t>
+        </is>
+      </c>
+      <c r="D41">
+        <v>10</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0.9</v>
+      </c>
+      <c r="H41">
+        <v>0.1</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
       </c>
       <c r="J41">
-        <v>224429</v>
+        <v>184597</v>
       </c>
       <c r="K41">
-        <v>0.336</v>
+        <v>0</v>
       </c>
       <c r="L41">
         <v>0</v>
       </c>
       <c r="M41">
-        <v>0.336</v>
+        <v>0</v>
       </c>
       <c r="N41">
-        <v>0.664</v>
+        <v>1</v>
+      </c>
+      <c r="O41" t="b">
+        <v>1</v>
+      </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>mark application issue: actual mark applied was not the intended mark applied</t>
+        </is>
       </c>
     </row>
     <row r="42">
       <c r="A42">
-        <v>2014</v>
+        <v>2020</v>
+      </c>
+      <c r="B42">
+        <v>422512</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Not Marked</t>
+        </is>
+      </c>
+      <c r="D42">
+        <v>10</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
       </c>
       <c r="J42">
-        <v>237435</v>
+        <v>422512</v>
       </c>
       <c r="K42">
-        <v>0.158</v>
+        <v>0</v>
       </c>
       <c r="L42">
         <v>0</v>
       </c>
       <c r="M42">
-        <v>0.158</v>
+        <v>0</v>
       </c>
       <c r="N42">
-        <v>0.842</v>
+        <v>1</v>
+      </c>
+      <c r="O42" t="b">
+        <v>1</v>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>mark application issue: actual mark applied was not the intended mark applied</t>
+        </is>
       </c>
     </row>
     <row r="43">
       <c r="A43">
-        <v>2016</v>
+        <v>2021</v>
+      </c>
+      <c r="B43">
+        <v>500039</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Marked</t>
+        </is>
+      </c>
+      <c r="D43">
+        <v>9</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
       </c>
       <c r="J43">
-        <v>542856</v>
+        <v>500039</v>
       </c>
       <c r="K43">
-        <v>0.089</v>
+        <v>0.075</v>
       </c>
       <c r="L43">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="M43">
-        <v>0.089</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="N43">
-        <v>0.911</v>
+        <v>0.914</v>
+      </c>
+      <c r="O43" t="b">
+        <v>1</v>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
       </c>
     </row>
     <row r="44">
       <c r="A44">
         <v>2022</v>
       </c>
+      <c r="D44">
+        <v>50</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
       <c r="J44">
         <v>478224</v>
       </c>
@@ -1646,6 +2042,16 @@
       </c>
       <c r="N44">
         <v>0.826</v>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>mark application issue: actual mark applied was not the intended mark applied</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
push marks by BY outputs
</commit_message>
<xml_diff>
--- a/outputs/R_OUT - San Juan mark history by BROOD YEAR.xlsx
+++ b/outputs/R_OUT - San Juan mark history by BROOD YEAR.xlsx
@@ -1,21 +1,125 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAVIDSONKA\Documents\ANALYSIS\Area20\A20\outputs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68754CE-0AB1-472A-8CB2-66D910E46A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="31">
+  <si>
+    <t>BROOD YEAR</t>
+  </si>
+  <si>
+    <t>TM_release</t>
+  </si>
+  <si>
+    <t>TM_read_status</t>
+  </si>
+  <si>
+    <t>n_submitted_refSpec_by_BY</t>
+  </si>
+  <si>
+    <t>TM Quality (%): NA</t>
+  </si>
+  <si>
+    <t>TM Quality (%): Unknown</t>
+  </si>
+  <si>
+    <t>TM Quality (%): Good</t>
+  </si>
+  <si>
+    <t>TM Quality (%): Acceptable</t>
+  </si>
+  <si>
+    <t>TM Quality (%): Poor</t>
+  </si>
+  <si>
+    <t>SEP_released</t>
+  </si>
+  <si>
+    <t>CWT</t>
+  </si>
+  <si>
+    <t>AD-only</t>
+  </si>
+  <si>
+    <t>mark rate</t>
+  </si>
+  <si>
+    <t>unmark/untag</t>
+  </si>
+  <si>
+    <t>total_rel_check</t>
+  </si>
+  <si>
+    <t>PBT</t>
+  </si>
+  <si>
+    <t>TM_comments</t>
+  </si>
+  <si>
+    <t>Marked</t>
+  </si>
+  <si>
+    <t>READS WERE 2:1.4+2.2 FOR 16 SAMPLES</t>
+  </si>
+  <si>
+    <t>NO REFERENCE SAMPLES.   RELEASE OF PINHEADS RESULTING FROM POOR FEED QUALITY-EWOS / NO REFERENCE SAMPLES.   FED FRY RELEASE, NO REFERENCE SAMPLES.</t>
+  </si>
+  <si>
+    <t>NO SAMPLE RECEIVED</t>
+  </si>
+  <si>
+    <t>12 HOUR THERMAL CYCLE NO SAMPLE RECEIVED</t>
+  </si>
+  <si>
+    <t>NO SAMPLE 12 HOUR THERMAL CYCLE</t>
+  </si>
+  <si>
+    <t>NO REFERENCE SAMPLE. THERMAL RECORDS PROVIDED BY HATCHERY</t>
+  </si>
+  <si>
+    <t>NO SAMPLE BUT THERMAL RECORDS(COHO POSSIBLY INCIDENTALLY MARKED)</t>
+  </si>
+  <si>
+    <t>Not Marked</t>
+  </si>
+  <si>
+    <t>FOUR MILE HATCHERY NO SAMPLE - MAURICE TREMBLAY NOT MARKED THIS YEAR DUE TO WATER TEMPERATURE ISSUES (SEE NOCN09115 AND NOCN09103)1,038,800 NOT THERMALLY MARKED.</t>
+  </si>
+  <si>
+    <t>mark application issue: actual mark applied was not the intended mark applied</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -31,13 +135,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,20 +166,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -109,7 +241,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -141,9 +273,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,6 +325,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,124 +518,121 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:XFD42"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="45.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>BROOD YEAR</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>TM_release</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>TM_read_status</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>n_submitted_refSpec_by_BY</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>TM Quality (%): NA</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>TM Quality (%): Unknown</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>TM Quality (%): Good</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>TM Quality (%): Acceptable</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>TM Quality (%): Poor</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>SEP_released</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>CWT</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>AD-only</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>mark rate</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>unmark/untag</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>total_rel_check</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>PBT</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>TM_comments</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1979</v>
       </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
       <c r="J2">
         <v>39555</v>
       </c>
       <c r="K2">
-        <v>0.989</v>
+        <v>0.98899999999999999</v>
       </c>
       <c r="L2">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="M2">
-        <v>0.994</v>
+        <v>0.99399999999999999</v>
       </c>
       <c r="N2">
-        <v>0.006</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1980</v>
       </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
       <c r="J3">
         <v>5560</v>
       </c>
@@ -484,10 +649,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1981</v>
       </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
       <c r="J4">
         <v>187527</v>
       </c>
@@ -498,36 +668,46 @@
         <v>0.03</v>
       </c>
       <c r="M4">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N4">
         <v>0.45</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1982</v>
       </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
       <c r="J5">
         <v>148677</v>
       </c>
       <c r="K5">
-        <v>0.335</v>
+        <v>0.33500000000000002</v>
       </c>
       <c r="L5">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="M5">
-        <v>0.348</v>
+        <v>0.34799999999999998</v>
       </c>
       <c r="N5">
-        <v>0.652</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>0.65200000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1983</v>
       </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
       <c r="J6">
         <v>99452</v>
       </c>
@@ -544,10 +724,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1984</v>
       </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
       <c r="J7">
         <v>367000</v>
       </c>
@@ -564,10 +749,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1985</v>
       </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
       <c r="J8">
         <v>29700</v>
       </c>
@@ -584,10 +774,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1986</v>
       </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
       <c r="J9">
         <v>300325</v>
       </c>
@@ -604,30 +799,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1987</v>
       </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
       <c r="J10">
         <v>711091</v>
       </c>
       <c r="K10">
-        <v>0.147</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>0.148</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="N10">
-        <v>0.852</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>0.85199999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1988</v>
       </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
       <c r="J11">
         <v>678464</v>
       </c>
@@ -635,19 +840,24 @@
         <v>0.153</v>
       </c>
       <c r="L11">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="M11">
         <v>0.155</v>
       </c>
       <c r="N11">
-        <v>0.845</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>0.84499999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1990</v>
       </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
       <c r="J12">
         <v>158990</v>
       </c>
@@ -664,10 +874,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1991</v>
       </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
       <c r="J13">
         <v>625000</v>
       </c>
@@ -684,70 +899,90 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1992</v>
       </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
       <c r="J14">
         <v>353071</v>
       </c>
       <c r="K14">
-        <v>0.385</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>0.385</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="N14">
-        <v>0.615</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>0.61499999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1993</v>
       </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
       <c r="J15">
         <v>1130250</v>
       </c>
       <c r="K15">
-        <v>0.045</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>0.045</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="N15">
-        <v>0.955</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>0.95499999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1994</v>
       </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
       <c r="J16">
         <v>670000</v>
       </c>
       <c r="K16">
-        <v>0.076</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>0.076</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="N16">
-        <v>0.924</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>0.92400000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1995</v>
       </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
       <c r="J17">
         <v>600000</v>
       </c>
@@ -764,10 +999,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1996</v>
       </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
       <c r="J18">
         <v>410000</v>
       </c>
@@ -784,10 +1024,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1997</v>
       </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
       <c r="J19">
         <v>275000</v>
       </c>
@@ -804,10 +1049,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1998</v>
       </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
       <c r="J20">
         <v>1275000</v>
       </c>
@@ -824,128 +1074,132 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1999</v>
       </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
       <c r="J21">
         <v>850000</v>
       </c>
       <c r="K21">
-        <v>0.08799999999999999</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21">
-        <v>0.089</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="N21">
-        <v>0.911</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>0.91100000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2000</v>
       </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
       <c r="J22">
         <v>224429</v>
       </c>
       <c r="K22">
-        <v>0.336</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="L22">
         <v>0</v>
       </c>
       <c r="M22">
-        <v>0.336</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="N22">
-        <v>0.664</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>0.66400000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2001</v>
       </c>
       <c r="B23">
         <v>785000</v>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
+      <c r="C23" t="s">
+        <v>17</v>
       </c>
       <c r="D23">
         <v>16</v>
       </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
+      <c r="E23" s="4">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4">
+        <v>1</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0</v>
+      </c>
+      <c r="I23" s="4">
         <v>0</v>
       </c>
       <c r="J23">
         <v>785000</v>
       </c>
       <c r="K23">
-        <v>0.096</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="L23">
         <v>0</v>
       </c>
       <c r="M23">
-        <v>0.096</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="N23">
-        <v>0.904</v>
+        <v>0.90400000000000003</v>
       </c>
       <c r="O23" t="b">
         <v>1</v>
       </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>READS WERE 2:1.4+2.2 FOR 16 SAMPLES</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
+      <c r="Q23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2002</v>
       </c>
       <c r="B24">
         <v>772052</v>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
+      <c r="C24" t="s">
+        <v>17</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
+      <c r="E24" s="4">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4">
+        <v>1</v>
+      </c>
+      <c r="G24" s="4">
+        <v>0</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0</v>
+      </c>
+      <c r="I24" s="4">
         <v>0</v>
       </c>
       <c r="J24">
@@ -966,40 +1220,36 @@
       <c r="O24" t="b">
         <v>1</v>
       </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>NO REFERENCE SAMPLES.   RELEASE OF PINHEADS RESULTING FROM POOR FEED QUALITY-EWOS / NO REFERENCE SAMPLES.   FED FRY RELEASE, NO REFERENCE SAMPLES.</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
+      <c r="Q24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2003</v>
       </c>
       <c r="B25">
         <v>1074172</v>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
+      <c r="C25" t="s">
+        <v>17</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25">
+      <c r="E25" s="4">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
+        <v>1</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0</v>
+      </c>
+      <c r="I25" s="4">
         <v>0</v>
       </c>
       <c r="J25">
@@ -1020,40 +1270,36 @@
       <c r="O25" t="b">
         <v>1</v>
       </c>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>NO SAMPLE RECEIVED</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
+      <c r="Q25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2004</v>
       </c>
       <c r="B26">
         <v>1000000</v>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
+      <c r="C26" t="s">
+        <v>17</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
+      <c r="E26" s="4">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4">
+        <v>1</v>
+      </c>
+      <c r="G26" s="4">
+        <v>0</v>
+      </c>
+      <c r="H26" s="4">
+        <v>0</v>
+      </c>
+      <c r="I26" s="4">
         <v>0</v>
       </c>
       <c r="J26">
@@ -1074,40 +1320,36 @@
       <c r="O26" t="b">
         <v>1</v>
       </c>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>12 HOUR THERMAL CYCLE NO SAMPLE RECEIVED</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
+      <c r="Q26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2005</v>
       </c>
       <c r="B27">
         <v>373275</v>
       </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
+      <c r="C27" t="s">
+        <v>17</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
+      <c r="E27" s="4">
+        <v>0</v>
+      </c>
+      <c r="F27" s="4">
+        <v>1</v>
+      </c>
+      <c r="G27" s="4">
+        <v>0</v>
+      </c>
+      <c r="H27" s="4">
+        <v>0</v>
+      </c>
+      <c r="I27" s="4">
         <v>0</v>
       </c>
       <c r="J27">
@@ -1128,40 +1370,36 @@
       <c r="O27" t="b">
         <v>1</v>
       </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>12 HOUR THERMAL CYCLE NO SAMPLE RECEIVED</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
+      <c r="Q27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2006</v>
       </c>
       <c r="B28">
         <v>985155</v>
       </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
+      <c r="C28" t="s">
+        <v>17</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28">
+      <c r="E28" s="4">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4">
+        <v>1</v>
+      </c>
+      <c r="G28" s="4">
+        <v>0</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0</v>
+      </c>
+      <c r="I28" s="4">
         <v>0</v>
       </c>
       <c r="J28">
@@ -1182,40 +1420,36 @@
       <c r="O28" t="b">
         <v>1</v>
       </c>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>NO SAMPLE 12 HOUR THERMAL CYCLE</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
+      <c r="Q28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2007</v>
       </c>
       <c r="B29">
         <v>518510</v>
       </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
+      <c r="C29" t="s">
+        <v>17</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
+      <c r="E29" s="4">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4">
+        <v>1</v>
+      </c>
+      <c r="G29" s="4">
+        <v>0</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0</v>
+      </c>
+      <c r="I29" s="4">
         <v>0</v>
       </c>
       <c r="J29">
@@ -1236,40 +1470,36 @@
       <c r="O29" t="b">
         <v>1</v>
       </c>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>NO REFERENCE SAMPLE. THERMAL RECORDS PROVIDED BY HATCHERY</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
+      <c r="Q29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2008</v>
       </c>
       <c r="B30">
         <v>945650</v>
       </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
+      <c r="C30" t="s">
+        <v>17</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30">
+      <c r="E30" s="4">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4">
+        <v>1</v>
+      </c>
+      <c r="G30" s="4">
+        <v>0</v>
+      </c>
+      <c r="H30" s="4">
+        <v>0</v>
+      </c>
+      <c r="I30" s="4">
         <v>0</v>
       </c>
       <c r="J30">
@@ -1290,40 +1520,36 @@
       <c r="O30" t="b">
         <v>1</v>
       </c>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>NO SAMPLE BUT THERMAL RECORDS(COHO POSSIBLY INCIDENTALLY MARKED)</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
+      <c r="Q30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2009</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Not Marked</t>
-        </is>
+      <c r="C31" t="s">
+        <v>25</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="I31">
+      <c r="E31" s="4">
+        <v>1</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0</v>
+      </c>
+      <c r="G31" s="4">
+        <v>0</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0</v>
+      </c>
+      <c r="I31" s="4">
         <v>0</v>
       </c>
       <c r="J31">
@@ -1344,40 +1570,36 @@
       <c r="O31" t="b">
         <v>0</v>
       </c>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>FOUR MILE HATCHERY NO SAMPLE - MAURICE TREMBLAY NOT MARKED THIS YEAR DUE TO WATER TEMPERATURE ISSUES (SEE NOCN09115 AND NOCN09103)1,038,800 NOT THERMALLY MARKED.</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
+      <c r="Q31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2010</v>
       </c>
       <c r="B32">
         <v>840000</v>
       </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
+      <c r="C32" t="s">
+        <v>17</v>
       </c>
       <c r="D32">
         <v>35</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="4">
         <v>0.2</v>
       </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
+      <c r="F32" s="4">
+        <v>0</v>
+      </c>
+      <c r="G32" s="4">
         <v>0.8</v>
       </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32">
+      <c r="H32" s="4">
+        <v>0</v>
+      </c>
+      <c r="I32" s="4">
         <v>0</v>
       </c>
       <c r="J32">
@@ -1398,40 +1620,36 @@
       <c r="O32" t="b">
         <v>1</v>
       </c>
-      <c r="Q32" t="inlineStr">
-        <is>
-          <t>mark application issue: actual mark applied was not the intended mark applied</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
+      <c r="Q32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2011</v>
       </c>
       <c r="B33">
         <v>245000</v>
       </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
+      <c r="C33" t="s">
+        <v>17</v>
       </c>
       <c r="D33">
         <v>15</v>
       </c>
-      <c r="E33">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="H33">
+      <c r="E33" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F33" s="4">
+        <v>0</v>
+      </c>
+      <c r="G33" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H33" s="4">
         <v>0.87</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="4">
         <v>0</v>
       </c>
       <c r="J33">
@@ -1452,40 +1670,36 @@
       <c r="O33" t="b">
         <v>1</v>
       </c>
-      <c r="Q33" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
+      <c r="Q33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2012</v>
       </c>
       <c r="B34">
         <v>1031800</v>
       </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
+      <c r="C34" t="s">
+        <v>17</v>
       </c>
       <c r="D34">
         <v>10</v>
       </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34">
+      <c r="E34" s="4">
+        <v>0</v>
+      </c>
+      <c r="F34" s="4">
+        <v>0</v>
+      </c>
+      <c r="G34" s="4">
+        <v>1</v>
+      </c>
+      <c r="H34" s="4">
+        <v>0</v>
+      </c>
+      <c r="I34" s="4">
         <v>0</v>
       </c>
       <c r="J34">
@@ -1506,91 +1720,83 @@
       <c r="O34" t="b">
         <v>1</v>
       </c>
-      <c r="Q34" t="inlineStr">
-        <is>
-          <t>mark application issue: actual mark applied was not the intended mark applied</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
+      <c r="Q34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2013</v>
       </c>
       <c r="B35">
         <v>319000</v>
       </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
+      <c r="C35" t="s">
+        <v>17</v>
       </c>
       <c r="D35">
         <v>10</v>
       </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
+      <c r="E35" s="4">
+        <v>0</v>
+      </c>
+      <c r="F35" s="4">
+        <v>0</v>
+      </c>
+      <c r="G35" s="4">
+        <v>1</v>
+      </c>
+      <c r="H35" s="4">
+        <v>0</v>
+      </c>
+      <c r="I35" s="4">
         <v>0</v>
       </c>
       <c r="J35">
         <v>319000</v>
       </c>
       <c r="K35">
-        <v>0.141</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="L35">
         <v>0</v>
       </c>
       <c r="M35">
-        <v>0.141</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="N35">
-        <v>0.859</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="O35" t="b">
         <v>1</v>
       </c>
-      <c r="Q35" t="inlineStr">
-        <is>
-          <t>mark application issue: actual mark applied was not the intended mark applied</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
+      <c r="Q35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2014</v>
       </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Not Marked</t>
-        </is>
+      <c r="C36" t="s">
+        <v>25</v>
       </c>
       <c r="D36">
         <v>17</v>
       </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="I36">
+      <c r="E36" s="4">
+        <v>1</v>
+      </c>
+      <c r="F36" s="4">
+        <v>0</v>
+      </c>
+      <c r="G36" s="4">
+        <v>0</v>
+      </c>
+      <c r="H36" s="4">
+        <v>0</v>
+      </c>
+      <c r="I36" s="4">
         <v>0</v>
       </c>
       <c r="J36">
@@ -1606,144 +1812,132 @@
         <v>0.158</v>
       </c>
       <c r="N36">
-        <v>0.842</v>
-      </c>
-      <c r="Q36" t="inlineStr">
-        <is>
-          <t>mark application issue: actual mark applied was not the intended mark applied</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2015</v>
       </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Not Marked</t>
-        </is>
+      <c r="C37" t="s">
+        <v>25</v>
       </c>
       <c r="D37">
         <v>10</v>
       </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37">
+      <c r="E37" s="4">
+        <v>1</v>
+      </c>
+      <c r="F37" s="4">
+        <v>0</v>
+      </c>
+      <c r="G37" s="4">
+        <v>0</v>
+      </c>
+      <c r="H37" s="4">
+        <v>0</v>
+      </c>
+      <c r="I37" s="4">
         <v>0</v>
       </c>
       <c r="J37">
         <v>219352</v>
       </c>
       <c r="K37">
-        <v>0.203</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="L37">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="M37">
-        <v>0.204</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="N37">
-        <v>0.796</v>
-      </c>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>mark application issue: actual mark applied was not the intended mark applied</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2016</v>
       </c>
       <c r="B38">
         <v>0</v>
       </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Not Marked</t>
-        </is>
+      <c r="C38" t="s">
+        <v>25</v>
       </c>
       <c r="D38">
         <v>10</v>
       </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38">
+      <c r="E38" s="4">
+        <v>1</v>
+      </c>
+      <c r="F38" s="4">
+        <v>0</v>
+      </c>
+      <c r="G38" s="4">
+        <v>0</v>
+      </c>
+      <c r="H38" s="4">
+        <v>0</v>
+      </c>
+      <c r="I38" s="4">
         <v>0</v>
       </c>
       <c r="J38">
         <v>542856</v>
       </c>
       <c r="K38">
-        <v>0.089</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="L38">
         <v>0</v>
       </c>
       <c r="M38">
-        <v>0.089</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="N38">
-        <v>0.911</v>
+        <v>0.91100000000000003</v>
       </c>
       <c r="O38" t="b">
         <v>0</v>
       </c>
-      <c r="Q38" t="inlineStr">
-        <is>
-          <t>mark application issue: actual mark applied was not the intended mark applied</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
+      <c r="Q38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2017</v>
       </c>
       <c r="B39">
         <v>249899</v>
       </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Not Marked</t>
-        </is>
+      <c r="C39" t="s">
+        <v>25</v>
       </c>
       <c r="D39">
         <v>10</v>
       </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39">
+      <c r="E39" s="4">
+        <v>1</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0</v>
+      </c>
+      <c r="G39" s="4">
+        <v>0</v>
+      </c>
+      <c r="H39" s="4">
+        <v>0</v>
+      </c>
+      <c r="I39" s="4">
         <v>0</v>
       </c>
       <c r="J39">
@@ -1753,56 +1947,50 @@
         <v>0.18</v>
       </c>
       <c r="L39">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="M39">
         <v>0.182</v>
       </c>
       <c r="N39">
-        <v>0.8179999999999999</v>
+        <v>0.81799999999999995</v>
       </c>
       <c r="O39" t="b">
         <v>1</v>
       </c>
-      <c r="P39" t="inlineStr">
-        <is>
-          <t>Incomplete</t>
-        </is>
-      </c>
-      <c r="Q39" t="inlineStr">
-        <is>
-          <t>mark application issue: actual mark applied was not the intended mark applied</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
+      <c r="P39" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2018</v>
       </c>
       <c r="B40">
         <v>66794</v>
       </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
+      <c r="C40" t="s">
+        <v>17</v>
       </c>
       <c r="D40">
         <v>10</v>
       </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
+      <c r="E40" s="4">
+        <v>0</v>
+      </c>
+      <c r="F40" s="4">
+        <v>0</v>
+      </c>
+      <c r="G40" s="4">
+        <v>1</v>
+      </c>
+      <c r="H40" s="4">
+        <v>0</v>
+      </c>
+      <c r="I40" s="4">
         <v>0</v>
       </c>
       <c r="J40">
@@ -1823,40 +2011,36 @@
       <c r="O40" t="b">
         <v>1</v>
       </c>
-      <c r="Q40" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
+      <c r="Q40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2019</v>
       </c>
       <c r="B41">
         <v>184597</v>
       </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
+      <c r="C41" t="s">
+        <v>17</v>
       </c>
       <c r="D41">
         <v>10</v>
       </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
+      <c r="E41" s="4">
+        <v>0</v>
+      </c>
+      <c r="F41" s="4">
+        <v>0</v>
+      </c>
+      <c r="G41" s="4">
         <v>0.9</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="4">
         <v>0.1</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="4">
         <v>0</v>
       </c>
       <c r="J41">
@@ -1877,45 +2061,39 @@
       <c r="O41" t="b">
         <v>1</v>
       </c>
-      <c r="P41" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
-      <c r="Q41" t="inlineStr">
-        <is>
-          <t>mark application issue: actual mark applied was not the intended mark applied</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
+      <c r="P41" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2020</v>
       </c>
       <c r="B42">
         <v>422512</v>
       </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Not Marked</t>
-        </is>
+      <c r="C42" t="s">
+        <v>25</v>
       </c>
       <c r="D42">
         <v>10</v>
       </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42">
+      <c r="E42" s="4">
+        <v>1</v>
+      </c>
+      <c r="F42" s="4">
+        <v>0</v>
+      </c>
+      <c r="G42" s="4">
+        <v>0</v>
+      </c>
+      <c r="H42" s="4">
+        <v>0</v>
+      </c>
+      <c r="I42" s="4">
         <v>0</v>
       </c>
       <c r="J42">
@@ -1936,122 +2114,108 @@
       <c r="O42" t="b">
         <v>1</v>
       </c>
-      <c r="P42" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>mark application issue: actual mark applied was not the intended mark applied</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
+      <c r="P42" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2021</v>
       </c>
       <c r="B43">
         <v>500039</v>
       </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>Marked</t>
-        </is>
+      <c r="C43" t="s">
+        <v>17</v>
       </c>
       <c r="D43">
         <v>9</v>
       </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-      <c r="I43">
+      <c r="E43" s="4">
+        <v>0</v>
+      </c>
+      <c r="F43" s="4">
+        <v>0</v>
+      </c>
+      <c r="G43" s="4">
+        <v>0</v>
+      </c>
+      <c r="H43" s="4">
+        <v>0</v>
+      </c>
+      <c r="I43" s="4">
         <v>1</v>
       </c>
       <c r="J43">
         <v>500039</v>
       </c>
       <c r="K43">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="L43">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="M43">
-        <v>0.08599999999999999</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="N43">
-        <v>0.914</v>
+        <v>0.91400000000000003</v>
       </c>
       <c r="O43" t="b">
         <v>1</v>
       </c>
-      <c r="P43" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
-      <c r="Q43" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
+      <c r="P43" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2022</v>
       </c>
       <c r="D44">
         <v>50</v>
       </c>
-      <c r="E44">
-        <v>1</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
-      <c r="H44">
-        <v>0</v>
-      </c>
-      <c r="I44">
+      <c r="E44" s="4">
+        <v>1</v>
+      </c>
+      <c r="F44" s="4">
+        <v>0</v>
+      </c>
+      <c r="G44" s="4">
+        <v>0</v>
+      </c>
+      <c r="H44" s="4">
+        <v>0</v>
+      </c>
+      <c r="I44" s="4">
         <v>0</v>
       </c>
       <c r="J44">
         <v>478224</v>
       </c>
       <c r="K44">
-        <v>0.174</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="L44">
         <v>0</v>
       </c>
       <c r="M44">
-        <v>0.174</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="N44">
-        <v>0.826</v>
-      </c>
-      <c r="P44" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
-      <c r="Q44" t="inlineStr">
-        <is>
-          <t>mark application issue: actual mark applied was not the intended mark applied</t>
-        </is>
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="P44" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update mark history by BY table output
</commit_message>
<xml_diff>
--- a/outputs/R_OUT - San Juan mark history by BROOD YEAR.xlsx
+++ b/outputs/R_OUT - San Juan mark history by BROOD YEAR.xlsx
@@ -1,26 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAVIDSONKA\Documents\ANALYSIS\Area20\A20\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68754CE-0AB1-472A-8CB2-66D910E46A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D68E1B3-3E7D-4CE2-B006-B7D7111B1B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="readme" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="49">
   <si>
     <t>BROOD YEAR</t>
   </si>
@@ -113,6 +127,60 @@
   </si>
   <si>
     <t>Full</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adult return year brood was collected from </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermal mark read status - marked or unmarked </t>
+  </si>
+  <si>
+    <t>Number of reference specimens used to assess quality and presence of a thermal mark</t>
+  </si>
+  <si>
+    <t>Proportion of reference specimens that returned a thermal mark quality of "NA"</t>
+  </si>
+  <si>
+    <t>Proportion of reference specimens that returned a thermal mark quality of "Unknown"</t>
+  </si>
+  <si>
+    <t>Proportion of reference specimens that returned a thermal mark quality of "Good"</t>
+  </si>
+  <si>
+    <t>Proportion of reference specimens that returned a thermal mark quality of "Acceptable"</t>
+  </si>
+  <si>
+    <t>Proportion of reference specimens that returned a thermal mark quality of "poor"</t>
+  </si>
+  <si>
+    <t>SEP's total release #s. Should == TM_release when TM_read_status=="Marked"</t>
+  </si>
+  <si>
+    <t>% releases with CWT</t>
+  </si>
+  <si>
+    <t>% of releases with an adipose clip</t>
+  </si>
+  <si>
+    <t>% of releases with some sort of identifying "SEP" mark, either CWT or adipose clip</t>
+  </si>
+  <si>
+    <t>% of releases that were unmarked and/or untagged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check that SEP releases == TM releases </t>
+  </si>
+  <si>
+    <t>Total number of hatchery juveniles released with thermal marks (TMs) - should be all juveniles released unless unmarked, in which case 0. When marked, this column should == "SEP_released". From otolith Manager database.</t>
+  </si>
+  <si>
+    <t>Were DNA collected for PBT? Was it a full sample?</t>
+  </si>
+  <si>
+    <t>Comments from NPAFC/Otolith Manager re: thermal mark quality/application issues. Note some years the applied mark was not the intended mark.</t>
   </si>
 </sst>
 </file>
@@ -199,9 +267,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -239,9 +307,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -274,26 +342,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -326,26 +377,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -521,8 +555,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:XFD42"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2221,4 +2256,164 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A23B3EED-607A-49F9-B19F-481FC9F2A56C}">
+  <dimension ref="A2:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>